<commit_message>
Automation Frameworks project updated
</commit_message>
<xml_diff>
--- a/Facebook/src/main/java/testData/FBtestData.xlsx
+++ b/Facebook/src/main/java/testData/FBtestData.xlsx
@@ -30,27 +30,20 @@
     <t>rigan</t>
   </si>
   <si>
-    <t>coolige</t>
+    <t>Jimy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,19 +63,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,7 +364,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -391,23 +380,23 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel data reader
</commit_message>
<xml_diff>
--- a/Facebook/src/main/java/testData/FBtestData.xlsx
+++ b/Facebook/src/main/java/testData/FBtestData.xlsx
@@ -30,7 +30,7 @@
     <t>rigan</t>
   </si>
   <si>
-    <t>Jimy</t>
+    <t>Jimy Carter</t>
   </si>
 </sst>
 </file>
@@ -362,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -374,29 +374,27 @@
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>